<commit_message>
update for 8 nodes
</commit_message>
<xml_diff>
--- a/8node_spain/output_a.xlsx
+++ b/8node_spain/output_a.xlsx
@@ -507,19 +507,19 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>0.0003978386713523962</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>2.689122860863488e-09</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>28.17704182552777</v>
+        <v>2.016951252558324</v>
       </c>
       <c r="H3" t="n">
-        <v>20.65093525419323</v>
+        <v>0.2031221295889138</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -535,7 +535,7 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>0.0003978386713523962</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
@@ -547,10 +547,10 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>23.21271746461933</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>16.19286578342044</v>
+        <v>0</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
@@ -578,10 +578,10 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>17.95850381196586</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>13.5511734331143</v>
+        <v>0</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
@@ -597,7 +597,7 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>2.689122860863488e-09</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
@@ -609,13 +609,13 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>18.54591470160023</v>
+        <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>23.46430640971666</v>
+        <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>8.255532014288399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -628,16 +628,16 @@
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>28.17704182552777</v>
+        <v>2.016951252558324</v>
       </c>
       <c r="D7" t="n">
-        <v>23.21271746461933</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>17.95850381196586</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>18.54591470160023</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -659,16 +659,16 @@
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>20.65093525419323</v>
+        <v>0.2031221295889138</v>
       </c>
       <c r="D8" t="n">
-        <v>16.19286578342044</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>13.5511734331143</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>23.46430640971666</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
@@ -677,7 +677,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>21.62916983090976</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -699,13 +699,13 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>8.255532014288399</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>21.62916983090976</v>
+        <v>0</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>

</xml_diff>